<commit_message>
grafikai javítások, alapértelmezett verseny az eredményfelvételnél
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,76 +544,82 @@
           <t>Verseny_ID</t>
         </is>
       </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Kategoria</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>6858</t>
+          <t>35.0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fekete Kálmán</t>
+          <t>Csefkó Pál</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Üllői Lövész Klub</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1998-01-07 00:00:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>36703219965</t>
-        </is>
-      </c>
+          <t>Csikóvári Para Sport Egyesület</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-09-13 20:47</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>999</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>777</t>
-        </is>
-      </c>
+      <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>VID_00001</t>
-        </is>
-      </c>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Dr. Seffer István</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Szent Hubertus Szituációs Lövészklub</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>o</t>
+        </is>
+      </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2025-09-14 22:14</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -627,7 +633,53 @@
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
-      <c r="V3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>VID_00001</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Vivert János</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Szent Hubertus Szituációs Lövészklub</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>VID_00001</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
keresés gyorsítás (500sor egyszerre renderelve)
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,11 +608,7 @@
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>o</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
@@ -680,10 +676,8 @@
       <c r="W4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="A5" t="n">
+        <v>35</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -724,6 +718,76 @@
       </c>
       <c r="W5" t="inlineStr"/>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>6858</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Fekete Kálmán</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Üllői Lövész Klub</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>VID_00001</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>VID_00001</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
azonosítók nem számként kezelése, UI bugfix, 1 :1 verseny versenyző kapcsolat kényszerítése
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -551,32 +551,14 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>35</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Csefkó Pál</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Csikóvári Para Sport Egyesület</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-09-13 20:47</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -719,10 +701,8 @@
       <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>6858</t>
-        </is>
+      <c r="A6" t="n">
+        <v>6858</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -760,9 +740,21 @@
       <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6865</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Gál László</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>B.T.K. Szituációs Lövész és Szabadidős Sportegyesület</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
@@ -781,11 +773,7 @@
       <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>VID_00001</t>
-        </is>
-      </c>
+      <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
requirements.txt telepítve, kód fut
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -551,14 +551,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="A2" t="n">
+        <v>980</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Turai Attila</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MTTSZ Béke Egyesület</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-09-15 19:12</t>
+        </is>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -740,10 +758,8 @@
       <c r="W6" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6865</t>
-        </is>
+      <c r="A7" t="n">
+        <v>6865</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
modified:   "database/Uzleti elv\303\241r\303\241sok.txt" 	modified:   database/error.log 	modified:   database/userDB.xlsx 	modified:   database/userDB.xlsx.bak 	modified:   database/versenyEredmenyek.xlsx 	modified:   database/versenyEredmenyek.xlsx.bak 	modified:   database/versenyekDB.xlsx 	modified:   database/versenyekDB.xlsx.bak
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -793,10 +793,8 @@
       <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>982</t>
-        </is>
+      <c r="A8" t="n">
+        <v>982</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>

</xml_diff>

<commit_message>
eredmenyek: automatikus verseny ID töltés
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,29 +552,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>980</v>
+        <v>25</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Turai Attila</t>
+          <t>Dr. Seffer István</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>MTTSZ Béke Egyesület</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
+          <t>Szent Hubertus Szituációs Lövészklub</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-09-15 19:12</t>
+          <t>2025-09-14 22:14</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -590,16 +586,20 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>VID_00001</t>
+        </is>
+      </c>
       <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dr. Seffer István</t>
+          <t>Vivert János</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -611,11 +611,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2025-09-14 22:14</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -638,23 +634,27 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Vivert János</t>
+          <t>Csefkó Pál</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Szent Hubertus Szituációs Lövészklub</t>
+          <t>Csikóvári Para Sport Egyesület</t>
         </is>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2025-09-13 20:47</t>
+        </is>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -677,27 +677,23 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>35</v>
+        <v>6858</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Csefkó Pál</t>
+          <t>Fekete Kálmán</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Csikóvári Para Sport Egyesület</t>
+          <t>Üllői Lövész Klub</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>2025-09-13 20:47</t>
-        </is>
-      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -719,19 +715,9 @@
       <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>6858</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Fekete Kálmán</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Üllői Lövész Klub</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -757,68 +743,6 @@
       </c>
       <c r="W6" t="inlineStr"/>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6865</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Gál László</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>B.T.K. Szituációs Lövész és Szabadidős Sportegyesület</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>982</v>
-      </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
üres sor visszatörölhető az eredményeknél
</commit_message>
<xml_diff>
--- a/database/versenyEredmenyek.xlsx
+++ b/database/versenyEredmenyek.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -715,9 +715,19 @@
       <c r="W5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
+      <c r="A6" t="n">
+        <v>6578</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Krokker Mihály</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Pandúr Lövész-Klub Sportegyesület</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
@@ -743,6 +753,39 @@
       </c>
       <c r="W6" t="inlineStr"/>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>8653</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>VID_00001</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>